<commit_message>
Modifs in database (2)
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_EV_Capacities.xlsx
+++ b/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_EV_Capacities.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\DispaSET-SideTools\Inputs\JRC_EU_TIMES\NearZeroCarbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{370049A5-FAA1-4E31-A04A-9B32D35B7D59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AC68B48-0B4A-4042-94DF-42AF08292998}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="2020" windowWidth="14720" windowHeight="7360" xr2:uid="{868663E0-8A9E-4DDF-A1D2-4800C4E89A44}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C211D56C-791B-4B16-92E8-F362ED356000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -188,11 +188,11 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -510,12 +510,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA465E7D-D8F1-44C6-ACAD-3EBDBB5D5D7D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F18D81F-3035-4673-85F9-C49CBFF1F28A}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -524,13 +522,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -539,10 +537,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="1">
-        <v>74.305999999999997</v>
+        <v>37.152999999999999</v>
       </c>
       <c r="C2" s="1">
-        <v>130.69200000000001</v>
+        <v>65.346000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -550,10 +548,10 @@
         <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>81.58</v>
+        <v>40.79</v>
       </c>
       <c r="C3" s="1">
-        <v>226.286</v>
+        <v>113.143</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -561,10 +559,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="1">
-        <v>28.422000000000001</v>
+        <v>14.211</v>
       </c>
       <c r="C4" s="1">
-        <v>68.819999999999993</v>
+        <v>34.409999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -572,10 +570,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="1">
-        <v>35.728000000000002</v>
+        <v>17.864000000000001</v>
       </c>
       <c r="C5" s="1">
-        <v>72.522000000000006</v>
+        <v>36.261000000000003</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -583,10 +581,10 @@
         <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>9.25</v>
+        <v>4.625</v>
       </c>
       <c r="C6" s="1">
-        <v>15.488</v>
+        <v>7.7439999999999998</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -594,10 +592,10 @@
         <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>45.143999999999998</v>
+        <v>22.571999999999999</v>
       </c>
       <c r="C7" s="1">
-        <v>90.36</v>
+        <v>45.18</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -605,10 +603,10 @@
         <v>9</v>
       </c>
       <c r="B8" s="1">
-        <v>390.536</v>
+        <v>195.268</v>
       </c>
       <c r="C8" s="1">
-        <v>673.02800000000002</v>
+        <v>336.51400000000001</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -616,10 +614,10 @@
         <v>10</v>
       </c>
       <c r="B9" s="1">
-        <v>45.322000000000003</v>
+        <v>22.661000000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>143.696</v>
+        <v>71.847999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -627,10 +625,10 @@
         <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>5.8239999999999998</v>
+        <v>2.9119999999999999</v>
       </c>
       <c r="C10" s="1">
-        <v>15.75</v>
+        <v>7.875</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -638,10 +636,10 @@
         <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>48.468000000000004</v>
+        <v>24.234000000000002</v>
       </c>
       <c r="C11" s="1">
-        <v>77.459999999999994</v>
+        <v>38.729999999999997</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -649,10 +647,10 @@
         <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>174.41399999999999</v>
+        <v>87.206999999999994</v>
       </c>
       <c r="C12" s="1">
-        <v>401.024</v>
+        <v>200.512</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -660,10 +658,10 @@
         <v>14</v>
       </c>
       <c r="B13" s="1">
-        <v>32.643999999999998</v>
+        <v>16.321999999999999</v>
       </c>
       <c r="C13" s="1">
-        <v>47.798000000000002</v>
+        <v>23.899000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -671,10 +669,10 @@
         <v>15</v>
       </c>
       <c r="B14" s="1">
-        <v>416.13799999999998</v>
+        <v>208.06899999999999</v>
       </c>
       <c r="C14" s="1">
-        <v>784.87800000000004</v>
+        <v>392.43900000000002</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -682,10 +680,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="1">
-        <v>19.094000000000001</v>
+        <v>9.5470000000000006</v>
       </c>
       <c r="C15" s="1">
-        <v>34.799999999999997</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -693,10 +691,10 @@
         <v>17</v>
       </c>
       <c r="B16" s="1">
-        <v>35.012</v>
+        <v>17.506</v>
       </c>
       <c r="C16" s="1">
-        <v>66.366</v>
+        <v>33.183</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -704,10 +702,10 @@
         <v>18</v>
       </c>
       <c r="B17" s="1">
-        <v>51.36</v>
+        <v>25.68</v>
       </c>
       <c r="C17" s="1">
-        <v>97.962000000000003</v>
+        <v>48.981000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -715,10 +713,10 @@
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>2.1080000000000001</v>
+        <v>1.054</v>
       </c>
       <c r="C18" s="1">
-        <v>4.1399999999999997</v>
+        <v>2.0699999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -726,10 +724,10 @@
         <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>320.14999999999998</v>
+        <v>160.07499999999999</v>
       </c>
       <c r="C19" s="1">
-        <v>608.73400000000004</v>
+        <v>304.36700000000002</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -737,10 +735,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="1">
-        <v>12.728</v>
+        <v>6.3639999999999999</v>
       </c>
       <c r="C20" s="1">
-        <v>28.341999999999999</v>
+        <v>14.170999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -748,10 +746,10 @@
         <v>22</v>
       </c>
       <c r="B21" s="1">
-        <v>26.31</v>
+        <v>13.154999999999999</v>
       </c>
       <c r="C21" s="1">
-        <v>44.878</v>
+        <v>22.439</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -759,10 +757,10 @@
         <v>23</v>
       </c>
       <c r="B22" s="1">
-        <v>7.8140000000000001</v>
+        <v>3.907</v>
       </c>
       <c r="C22" s="1">
-        <v>12.332000000000001</v>
+        <v>6.1660000000000004</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -770,10 +768,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>3.9460000000000002</v>
+        <v>1.9730000000000001</v>
       </c>
       <c r="C23" s="1">
-        <v>1.3979999999999999</v>
+        <v>0.69899999999999995</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -781,10 +779,10 @@
         <v>25</v>
       </c>
       <c r="B24" s="1">
-        <v>120.86799999999999</v>
+        <v>60.433999999999997</v>
       </c>
       <c r="C24" s="1">
-        <v>673.99199999999996</v>
+        <v>336.99599999999998</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -792,10 +790,10 @@
         <v>26</v>
       </c>
       <c r="B25" s="1">
-        <v>37.978000000000002</v>
+        <v>18.989000000000001</v>
       </c>
       <c r="C25" s="1">
-        <v>57.634</v>
+        <v>28.817</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -803,10 +801,10 @@
         <v>27</v>
       </c>
       <c r="B26" s="1">
-        <v>100.51600000000001</v>
+        <v>50.258000000000003</v>
       </c>
       <c r="C26" s="1">
-        <v>286.22000000000003</v>
+        <v>143.11000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -814,10 +812,10 @@
         <v>28</v>
       </c>
       <c r="B27" s="1">
-        <v>66.617999999999995</v>
+        <v>33.308999999999997</v>
       </c>
       <c r="C27" s="1">
-        <v>114.82599999999999</v>
+        <v>57.412999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -825,10 +823,10 @@
         <v>29</v>
       </c>
       <c r="B28" s="1">
-        <v>42.097999999999999</v>
+        <v>21.048999999999999</v>
       </c>
       <c r="C28" s="1">
-        <v>84.555999999999997</v>
+        <v>42.277999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -836,10 +834,10 @@
         <v>30</v>
       </c>
       <c r="B29" s="1">
-        <v>60.072000000000003</v>
+        <v>30.036000000000001</v>
       </c>
       <c r="C29" s="1">
-        <v>107.896</v>
+        <v>53.948</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -847,10 +845,10 @@
         <v>31</v>
       </c>
       <c r="B30" s="1">
-        <v>18.11</v>
+        <v>9.0549999999999997</v>
       </c>
       <c r="C30" s="1">
-        <v>28.667999999999999</v>
+        <v>14.334</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -858,10 +856,10 @@
         <v>32</v>
       </c>
       <c r="B31" s="1">
-        <v>13.036</v>
+        <v>6.5179999999999998</v>
       </c>
       <c r="C31" s="1">
-        <v>31.18</v>
+        <v>15.59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -869,10 +867,10 @@
         <v>33</v>
       </c>
       <c r="B32" s="1">
-        <v>287.47000000000003</v>
+        <v>143.73500000000001</v>
       </c>
       <c r="C32" s="1">
-        <v>826.95</v>
+        <v>413.47500000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed EV storage capacity
</commit_message>
<xml_diff>
--- a/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_EV_Capacities.xlsx
+++ b/Inputs/JRC_EU_TIMES/NearZeroCarbon/TIMES_EV_Capacities.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eva\Downloads\MASTER\TFE\DispaSET-SideTools\Inputs\JRC_EU_TIMES\NearZeroCarbon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10459618_polimi_it/Documents/Università/Tesi (OneDrive)/Final Simulations Dispa-SET/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AC68B48-0B4A-4042-94DF-42AF08292998}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5CB1E26-F717-4537-ACAF-A0B175724153}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C211D56C-791B-4B16-92E8-F362ED356000}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{ADFDABF0-C260-4C25-A473-7D87ED15857C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,15 +33,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+  <si>
+    <t>Process Description1  /  Commod Unit  /  Unit - capacity</t>
+  </si>
+  <si>
+    <t>Battery Charging Station</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>2030</t>
-  </si>
-  <si>
-    <t>2050</t>
+    <t>GW</t>
   </si>
   <si>
     <t>AT</t>
@@ -139,9 +147,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0.0"/>
-  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,16 +188,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -215,7 +223,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -510,371 +518,566 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F18D81F-3035-4673-85F9-C49CBFF1F28A}">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1EA875-11FD-4B86-B954-86975583FCBF}">
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="4.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
-        <v>37.152999999999999</v>
-      </c>
-      <c r="C2" s="1">
-        <v>65.346000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
-        <v>40.79</v>
-      </c>
-      <c r="C3" s="1">
-        <v>113.143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
-        <v>14.211</v>
-      </c>
-      <c r="C4" s="1">
-        <v>34.409999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="1">
+        <v>11.346</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="1">
-        <v>17.864000000000001</v>
-      </c>
-      <c r="C5" s="1">
-        <v>36.261000000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="1">
+        <v>13.922000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
-        <v>4.625</v>
-      </c>
-      <c r="C6" s="1">
-        <v>7.7439999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="1">
+        <v>7.0190000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="1">
-        <v>22.571999999999999</v>
-      </c>
-      <c r="C7" s="1">
-        <v>45.18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="1">
+        <v>9.2989999999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1">
-        <v>195.268</v>
-      </c>
-      <c r="C8" s="1">
-        <v>336.51400000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="1">
+        <v>1.573</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1">
-        <v>22.661000000000001</v>
-      </c>
-      <c r="C9" s="1">
-        <v>71.847999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="1">
+        <v>14.675000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1">
-        <v>2.9119999999999999</v>
-      </c>
-      <c r="C10" s="1">
-        <v>7.875</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="1">
+        <v>90.370999999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1">
-        <v>24.234000000000002</v>
-      </c>
-      <c r="C11" s="1">
-        <v>38.729999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
+      <c r="B12" s="1">
+        <v>5.7809999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
-        <v>87.206999999999994</v>
-      </c>
-      <c r="C12" s="1">
-        <v>200.512</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
+      <c r="B13" s="1">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="1">
-        <v>16.321999999999999</v>
-      </c>
-      <c r="C13" s="1">
-        <v>23.899000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="B14" s="1">
+        <v>11.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1">
-        <v>208.06899999999999</v>
-      </c>
-      <c r="C14" s="1">
-        <v>392.43900000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="1">
+        <v>65.012</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1">
-        <v>9.5470000000000006</v>
-      </c>
-      <c r="C15" s="1">
-        <v>17.399999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="B16" s="1">
+        <v>6.1159999999999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="1">
-        <v>17.506</v>
-      </c>
-      <c r="C16" s="1">
-        <v>33.183</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="1">
+        <v>79.816000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1">
-        <v>25.68</v>
-      </c>
-      <c r="C17" s="1">
-        <v>48.981000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="1">
+        <v>3.9990000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1">
-        <v>1.054</v>
-      </c>
-      <c r="C18" s="1">
-        <v>2.0699999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
+      <c r="B19" s="1">
+        <v>9.08</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1">
-        <v>160.07499999999999</v>
-      </c>
-      <c r="C19" s="1">
-        <v>304.36700000000002</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="B20" s="1">
+        <v>5.5309999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1">
-        <v>6.3639999999999999</v>
-      </c>
-      <c r="C20" s="1">
-        <v>14.170999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="4" t="s">
+      <c r="B21" s="1">
+        <v>0.499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="1">
-        <v>13.154999999999999</v>
-      </c>
-      <c r="C21" s="1">
-        <v>22.439</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="4" t="s">
+      <c r="B22" s="1">
+        <v>89.963999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="1">
-        <v>3.907</v>
-      </c>
-      <c r="C22" s="1">
-        <v>6.1660000000000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="1">
+        <v>4.2169999999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="1">
-        <v>1.9730000000000001</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0.69899999999999995</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="B24" s="1">
+        <v>1.254</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="1">
-        <v>60.433999999999997</v>
-      </c>
-      <c r="C24" s="1">
-        <v>336.99599999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="1">
+        <v>1.2170000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="1">
-        <v>18.989000000000001</v>
-      </c>
-      <c r="C25" s="1">
-        <v>28.817</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="1">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="1">
-        <v>50.258000000000003</v>
-      </c>
-      <c r="C26" s="1">
-        <v>143.11000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="4" t="s">
+      <c r="B27" s="1">
+        <v>18.559000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="1">
-        <v>33.308999999999997</v>
-      </c>
-      <c r="C27" s="1">
-        <v>57.412999999999997</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="B28" s="1">
+        <v>5.2930000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="1">
-        <v>21.048999999999999</v>
-      </c>
-      <c r="C28" s="1">
-        <v>42.277999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="1">
+        <v>62.695</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="1">
-        <v>30.036000000000001</v>
-      </c>
-      <c r="C29" s="1">
-        <v>53.948</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
+      <c r="B30" s="1">
+        <v>12.319000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="1">
-        <v>9.0549999999999997</v>
-      </c>
-      <c r="C30" s="1">
-        <v>14.334</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
+      <c r="B31" s="1">
+        <v>19.984999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="1">
-        <v>6.5179999999999998</v>
-      </c>
-      <c r="C31" s="1">
-        <v>15.59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
+      <c r="B32" s="1">
+        <v>10.635</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="1">
-        <v>143.73500000000001</v>
-      </c>
-      <c r="C32" s="1">
-        <v>413.47500000000002</v>
+      <c r="B33" s="1">
+        <v>2.8959999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1">
+        <v>6.0759999999999996</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1">
+        <v>71.914000000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100BA58F2CACE833A4EAC3C2718D7553EBC" ma:contentTypeVersion="13" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="bb63102ff0d9eda75d0b4de88b67103d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="7880897e-52c6-4ffd-85c8-5c6950347fc0" xmlns:ns4="8c824e80-41b8-4a07-a4d9-9d9814734933" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d343f4382375feb5aaefc2a566ff9801" ns3:_="" ns4:_="">
+    <xsd:import namespace="7880897e-52c6-4ffd-85c8-5c6950347fc0"/>
+    <xsd:import namespace="8c824e80-41b8-4a07-a4d9-9d9814734933"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharingHintHash" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns4:MediaServiceKeyPoints" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="7880897e-52c6-4ffd-85c8-5c6950347fc0" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithDetails" ma:index="8" nillable="true" ma:displayName="Condiviso con dettagli" ma:description="" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="SharedWithUsers" ma:index="9" nillable="true" ma:displayName="Condiviso con" ma:description="" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharingHintHash" ma:index="10" nillable="true" ma:displayName="Hash suggerimento condivisione" ma:description="" ma:hidden="true" ma:internalName="SharingHintHash" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="8c824e80-41b8-4a07-a4d9-9d9814734933" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="11" nillable="true" ma:displayName="MediaServiceMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="12" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:description="" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="13" nillable="true" ma:displayName="MediaServiceDateTaken" ma:description="" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="MediaServiceAutoTags" ma:description="" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="MediaServiceOCR" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="16" nillable="true" ma:displayName="MediaServiceLocation" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="17" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="19" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="20" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo di contenuto"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Titolo"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B05015A-249B-487F-8B04-DDAEF8E54C95}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7880897e-52c6-4ffd-85c8-5c6950347fc0"/>
+    <ds:schemaRef ds:uri="8c824e80-41b8-4a07-a4d9-9d9814734933"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48CC40A8-361F-47BA-A0C2-7B7B61A96AB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7CC47E11-9F3E-4622-A080-1A69DA245831}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>